<commit_message>
Updated Purchasing list, removed two components
</commit_message>
<xml_diff>
--- a/Component_Placement_Sheet.xlsx
+++ b/Component_Placement_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saxani/My Drive/CosmicWatch/GitHub/CosmicWatch-Desktop-Muon-Detector-v3X/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2136ED1-B492-6B49-A5CD-359D6462D29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC41F7A-15E4-C34A-B80D-D726C240DA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="24540" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="209">
   <si>
     <t>1k</t>
   </si>
@@ -327,9 +327,6 @@
   </si>
   <si>
     <t>CAP CER 10000PF 50V X7R 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 pin SMT (on SiPM board) </t>
   </si>
   <si>
     <t xml:space="preserve">2x3 pins </t>
@@ -357,9 +354,6 @@
     <t>CONN HEADER SMD 6POS 2.54MM</t>
   </si>
   <si>
-    <t>2x screws to mount the standoffs to SiPM board</t>
-  </si>
-  <si>
     <t>0-80 Thread Size, 1/4" Long</t>
   </si>
   <si>
@@ -511,15 +505,9 @@
     <t>RES SMD 1.3K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>R24,R12,R22,R19,R17,R21,R25,R30</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>C2,C3,C19,C17,C20</t>
-  </si>
-  <si>
     <t>154k</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
     <t>R7</t>
   </si>
   <si>
-    <t>R26, R10, R14</t>
-  </si>
-  <si>
     <t>C5,C13</t>
   </si>
   <si>
@@ -586,12 +571,6 @@
     <t>Laser cut by uploading Enclosures/Faceplates.zip file to elecrow.com</t>
   </si>
   <si>
-    <t>Uses same pins as BMP280, although on other side of board. Careful with direction. Sensor faces into the PCB.</t>
-  </si>
-  <si>
-    <t>Bottom side of board. Align VCC pin.</t>
-  </si>
-  <si>
     <t>CosmicWatch v3X Componet Placement Sheet</t>
   </si>
   <si>
@@ -607,9 +586,6 @@
     <t>100</t>
   </si>
   <si>
-    <t>R8,R18,R23,R28,R29, R9</t>
-  </si>
-  <si>
     <t>Drill holes for #2 screws using #48 bit, diameter = 1.93mm, 30mm apart, in a square.</t>
   </si>
   <si>
@@ -625,9 +601,6 @@
     <t>MICROFC-60035-SMT-TR</t>
   </si>
   <si>
-    <t>Very important, Note direction. Find pin 1</t>
-  </si>
-  <si>
     <t>Request for a 2506-2.9 split body case</t>
   </si>
   <si>
@@ -653,6 +626,42 @@
   </si>
   <si>
     <t>Alt Link</t>
+  </si>
+  <si>
+    <t>R12,R24,R22,R19,R17,R30,R21,R25</t>
+  </si>
+  <si>
+    <t>C3,C2,C19,C17,C20</t>
+  </si>
+  <si>
+    <t>R9,R29,R28,R8,R18,R23</t>
+  </si>
+  <si>
+    <t>R10,R26,R14</t>
+  </si>
+  <si>
+    <t>Bottom side of board. FLAT AGAINST BOARD. Align VCC pin.</t>
+  </si>
+  <si>
+    <t>Uses same pins as BMP280, although on top side of board. Careful with direction. Sensor faces into the PCB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2: LED 3mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5: LED 5mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P7: 6 pin SMT (on SiPM board) </t>
+  </si>
+  <si>
+    <t>Very important, Note direction. Find pin 1 from datasheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Screw through SiPM side in board. 2 others mount to Main PCB. </t>
+  </si>
+  <si>
+    <t>4x screws to mount the standoffs to SiPM board</t>
   </si>
 </sst>
 </file>
@@ -3072,8 +3081,8 @@
   </sheetPr>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3093,7 +3102,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3119,10 +3128,10 @@
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>37</v>
@@ -3137,19 +3146,19 @@
         <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -3159,10 +3168,10 @@
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
       <c r="I4" s="23" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
@@ -3170,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>0</v>
@@ -3181,7 +3190,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="22">
@@ -3196,18 +3205,18 @@
         <v>2</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="22">
@@ -3233,7 +3242,7 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="22">
@@ -3248,7 +3257,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C8" s="8">
         <v>100</v>
@@ -3259,7 +3268,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="22">
@@ -3274,7 +3283,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -3287,7 +3296,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="22">
@@ -3302,7 +3311,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>51</v>
@@ -3313,7 +3322,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="22">
@@ -3339,7 +3348,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="22">
@@ -3354,7 +3363,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>44</v>
@@ -3365,7 +3374,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="22">
@@ -3383,7 +3392,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6" t="s">
@@ -3391,7 +3400,7 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="22">
@@ -3419,7 +3428,7 @@
         <v>49</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="22">
@@ -3441,13 +3450,13 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="6" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="22">
@@ -3459,7 +3468,7 @@
     </row>
     <row r="16" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
@@ -3487,7 +3496,7 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="22">
@@ -3513,7 +3522,7 @@
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="22">
@@ -3541,7 +3550,7 @@
         <v>50</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="22">
@@ -3563,13 +3572,13 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="22">
@@ -3587,17 +3596,17 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="22">
@@ -3619,13 +3628,13 @@
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="22">
@@ -3653,7 +3662,7 @@
         <v>50</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="22">
@@ -3678,10 +3687,10 @@
         <v>58</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="22">
@@ -3693,7 +3702,7 @@
     </row>
     <row r="25" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -3710,7 +3719,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>21</v>
@@ -3721,7 +3730,7 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="22">
@@ -3736,18 +3745,18 @@
         <v>21</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="22">
@@ -3773,7 +3782,7 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="22">
@@ -3788,18 +3797,18 @@
         <v>23</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="22">
@@ -3814,7 +3823,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>63</v>
@@ -3825,7 +3834,7 @@
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="22">
@@ -3853,7 +3862,7 @@
         <v>69</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H31" s="20"/>
       <c r="I31" s="22">
@@ -3881,10 +3890,10 @@
         <v>68</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I32" s="22">
         <v>2.48</v>
@@ -3895,7 +3904,7 @@
     </row>
     <row r="33" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -3919,16 +3928,16 @@
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>72</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I34" s="22">
         <v>0.33</v>
@@ -3956,7 +3965,7 @@
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I35" s="22">
         <v>0.45</v>
@@ -3983,10 +3992,10 @@
         <v>76</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I36" s="24">
         <f>6.89/10</f>
@@ -4011,13 +4020,13 @@
         <v>79</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I37" s="22">
         <f>7.39/5</f>
@@ -4033,20 +4042,20 @@
         <v>32</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H38" s="20"/>
       <c r="I38" s="22">
@@ -4062,7 +4071,7 @@
         <v>33</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>80</v>
+        <v>203</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>80</v>
@@ -4075,7 +4084,7 @@
         <v>82</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="24">
@@ -4092,7 +4101,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>83</v>
@@ -4105,7 +4114,7 @@
         <v>85</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="22">
@@ -4135,10 +4144,10 @@
         <v>92</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I41" s="22">
         <v>5</v>
@@ -4165,10 +4174,10 @@
         <v>90</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I42" s="22">
         <f>7.29/6</f>
@@ -4209,7 +4218,7 @@
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="22">
@@ -4235,7 +4244,7 @@
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="22">
@@ -4250,7 +4259,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>44</v>
@@ -4261,7 +4270,7 @@
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="22">
@@ -4276,18 +4285,18 @@
         <v>40</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="22">
@@ -4302,10 +4311,10 @@
         <v>41</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="6" t="s">
@@ -4313,7 +4322,7 @@
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="22">
@@ -4328,20 +4337,20 @@
         <v>42</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="22">
@@ -4359,17 +4368,17 @@
         <v>2</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="15" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H50" s="20"/>
       <c r="I50" s="22">
@@ -4384,20 +4393,20 @@
         <v>44</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="22">
@@ -4412,20 +4421,20 @@
         <v>45</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="22">
@@ -4439,7 +4448,7 @@
     </row>
     <row r="53" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="37"/>
       <c r="C53" s="37"/>
@@ -4456,18 +4465,18 @@
         <v>46</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="15" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H54" s="20"/>
       <c r="I54" s="22">
@@ -4482,20 +4491,20 @@
         <v>47</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H55" s="20"/>
       <c r="I55" s="22">
@@ -4510,18 +4519,18 @@
         <v>48</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H56" s="21"/>
       <c r="I56" s="22">
@@ -4536,20 +4545,20 @@
         <v>49</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="24">
@@ -4565,20 +4574,20 @@
         <v>50</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H58" s="20"/>
       <c r="I58" s="24">
@@ -4595,20 +4604,20 @@
         <v>51</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H59" s="20"/>
       <c r="I59" s="22">
@@ -4623,23 +4632,23 @@
         <v>52</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I60" s="24">
         <f>8.89/6</f>
@@ -4655,20 +4664,20 @@
         <v>53</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H61" s="21"/>
       <c r="I61" s="22">
@@ -4683,21 +4692,21 @@
         <v>54</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I62" s="24">
         <f>3.99/100</f>
@@ -4713,21 +4722,21 @@
         <v>55</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I63" s="22">
         <f>6.09/20</f>
@@ -4743,21 +4752,21 @@
         <v>56</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I64" s="22">
         <f>11.39/100</f>
@@ -4773,20 +4782,20 @@
         <v>57</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H65" s="21"/>
       <c r="I65" s="22">
@@ -4801,21 +4810,21 @@
         <v>58</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I66" s="22">
         <v>7.19</v>
@@ -4829,18 +4838,18 @@
         <v>59</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H67" s="18"/>
       <c r="I67" s="22">
@@ -4852,7 +4861,7 @@
     </row>
     <row r="68" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G68" s="16" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H68" s="16"/>
       <c r="I68" s="16">

</xml_diff>